<commit_message>
Added 'status' field to notification.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-backport-subscription-status.xlsx
+++ b/docs/StructureDefinition-backport-subscription-status.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$62</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="133">
   <si>
     <t>Path</t>
   </si>
@@ -247,7 +247,7 @@
     <t>Parameters.parameter</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
   <si>
     <t xml:space="preserve">BackboneElement
@@ -390,6 +390,33 @@
     <t>Only one level of nested parameters is allowed.</t>
   </si>
   <si>
+    <t>subscriptionUrl</t>
+  </si>
+  <si>
+    <t>subscription-url</t>
+  </si>
+  <si>
+    <t>subscriptionTopicUrl</t>
+  </si>
+  <si>
+    <t>subscription-topic-url</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/subscription-status</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/subscriptions-backport/ValueSet/backport-notification-type-value-set</t>
+  </si>
+  <si>
     <t>subscriptionEventCount</t>
   </si>
   <si>
@@ -404,27 +431,6 @@
   </si>
   <si>
     <t>bundle-event-count</t>
-  </si>
-  <si>
-    <t>subscriptionTopicUrl</t>
-  </si>
-  <si>
-    <t>subscription-topic-url</t>
-  </si>
-  <si>
-    <t>subscriptionUrl</t>
-  </si>
-  <si>
-    <t>subscription-url</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/subscriptions-backport/ValueSet/backport-notification-type-value-set</t>
   </si>
 </sst>
 </file>
@@ -573,7 +579,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK54"/>
+  <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2639,7 +2645,7 @@
         <v>47</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>121</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s" s="2">
         <v>107</v>
@@ -2932,14 +2938,14 @@
         <v>74</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>46</v>
@@ -3390,7 +3396,7 @@
         <v>38</v>
       </c>
       <c r="R27" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S27" t="s" s="2">
         <v>38</v>
@@ -3475,7 +3481,7 @@
         <v>47</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>121</v>
+        <v>60</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>107</v>
@@ -3768,14 +3774,14 @@
         <v>74</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>46</v>
@@ -4226,7 +4232,7 @@
         <v>38</v>
       </c>
       <c r="R35" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S35" t="s" s="2">
         <v>38</v>
@@ -4296,7 +4302,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>46</v>
@@ -4311,7 +4317,7 @@
         <v>47</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="K36" t="s" s="2">
         <v>107</v>
@@ -4344,13 +4350,11 @@
         <v>38</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X36" t="s" s="2">
-        <v>38</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="X36" s="2"/>
       <c r="Y36" t="s" s="2">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>38</v>
@@ -5062,7 +5066,7 @@
         <v>38</v>
       </c>
       <c r="R43" t="s" s="2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S43" t="s" s="2">
         <v>38</v>
@@ -5147,7 +5151,7 @@
         <v>47</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="K44" t="s" s="2">
         <v>107</v>
@@ -5180,13 +5184,11 @@
         <v>38</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X44" t="s" s="2">
-        <v>38</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="X44" s="2"/>
       <c r="Y44" t="s" s="2">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>38</v>
@@ -5898,7 +5900,7 @@
         <v>38</v>
       </c>
       <c r="R51" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="S51" t="s" s="2">
         <v>38</v>
@@ -5983,7 +5985,7 @@
         <v>47</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="K52" t="s" s="2">
         <v>107</v>
@@ -6016,11 +6018,13 @@
         <v>38</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="X52" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="Y52" t="s" s="2">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>38</v>
@@ -6269,8 +6273,844 @@
         <v>38</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="C55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F56" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" hidden="true">
+      <c r="A57" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="N57" s="2"/>
+      <c r="O57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="Q57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" hidden="true">
+      <c r="A58" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H58" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="I58" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="J58" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="O58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P58" s="2"/>
+      <c r="Q58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE58" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AF58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AI58" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK58" t="s" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" hidden="true">
+      <c r="A59" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="F59" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="J59" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P59" s="2"/>
+      <c r="Q59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R59" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="S59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE59" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AF59" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AG59" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AI59" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK59" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F60" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G60" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I60" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="J60" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="K60" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P60" s="2"/>
+      <c r="Q60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE60" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" hidden="true">
+      <c r="A61" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F61" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I61" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="J61" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="K61" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="N61" s="2"/>
+      <c r="O61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P61" s="2"/>
+      <c r="Q61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="N62" s="2"/>
+      <c r="O62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="S62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AK54">
+  <autoFilter ref="A1:AK62">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6280,7 +7120,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI53">
+  <conditionalFormatting sqref="A2:AI61">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updates to remove IG errors and warnings.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-backport-subscription-status.xlsx
+++ b/docs/StructureDefinition-backport-subscription-status.xlsx
@@ -264,7 +264,7 @@
 </t>
   </si>
   <si>
-    <t>Slice on name</t>
+    <t>Slice on parameter name</t>
   </si>
   <si>
     <t>open</t>
@@ -615,7 +615,7 @@
     <col min="25" max="25" width="83.515625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="23.43359375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
@@ -2557,10 +2557,10 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" t="s" s="2">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="R19" t="s" s="2">
-        <v>120</v>
+        <v>38</v>
       </c>
       <c r="S19" t="s" s="2">
         <v>38</v>
@@ -3393,10 +3393,10 @@
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" t="s" s="2">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="R27" t="s" s="2">
-        <v>122</v>
+        <v>38</v>
       </c>
       <c r="S27" t="s" s="2">
         <v>38</v>
@@ -4229,10 +4229,10 @@
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" t="s" s="2">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="R35" t="s" s="2">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="S35" t="s" s="2">
         <v>38</v>
@@ -5063,10 +5063,10 @@
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" t="s" s="2">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="R43" t="s" s="2">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="S43" t="s" s="2">
         <v>38</v>
@@ -5897,10 +5897,10 @@
       </c>
       <c r="P51" s="2"/>
       <c r="Q51" t="s" s="2">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="R51" t="s" s="2">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="S51" t="s" s="2">
         <v>38</v>
@@ -6733,10 +6733,10 @@
       </c>
       <c r="P59" s="2"/>
       <c r="Q59" t="s" s="2">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="R59" t="s" s="2">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="S59" t="s" s="2">
         <v>38</v>

</xml_diff>